<commit_message>
finish sub bab 5.2.3 waktu postingan
</commit_message>
<xml_diff>
--- a/ANALISIS.xlsx
+++ b/ANALISIS.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d6a266968836285/Documents/COURSE MATERIAL/KERJA PRAKTIK/LAPORAN-KP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2F1C2A6-858B-4D24-BFDF-9FC6532B93C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="129" documentId="8_{C2F1C2A6-858B-4D24-BFDF-9FC6532B93C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2637425C-48AD-4E10-AEE4-17E4C797F0CD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{A23BCB5B-6445-452F-AECE-183DD30B1911}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{A23BCB5B-6445-452F-AECE-183DD30B1911}"/>
   </bookViews>
   <sheets>
     <sheet name="EFEKTIVITAS KONTEN" sheetId="1" r:id="rId1"/>
     <sheet name="HITUNG EFEKTIVITAS KONTEN" sheetId="2" r:id="rId2"/>
+    <sheet name="FREKUENSI POSTINGAN" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="22">
   <si>
     <t>Kategori Konten</t>
   </si>
@@ -84,6 +85,24 @@
   <si>
     <t>NO</t>
   </si>
+  <si>
+    <t>Tanggal Posting</t>
+  </si>
+  <si>
+    <t>Jumlah Postingan</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>Desember</t>
+  </si>
+  <si>
+    <t>Januari</t>
+  </si>
+  <si>
+    <t>Februari</t>
+  </si>
 </sst>
 </file>
 
@@ -123,7 +142,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -179,11 +198,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -195,7 +236,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,7 +558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4C9485-0085-4ACC-A56D-43AABF5F9F6D}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
@@ -660,7 +706,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6C946BC-6785-47DB-89FD-92BF06E2F11F}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -2038,4 +2084,358 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{032A0377-CAA8-4CBF-91AC-C113C6EF723D}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>45616</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>45619</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>45620</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>45621</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>45623</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>45629</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>45630</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>45631</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>45633</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>45635</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>45636</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>45637</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>45638</v>
+      </c>
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>45642</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>45643</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>45644</v>
+      </c>
+      <c r="B17" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>45645</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
+        <v>45647</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
+        <v>45650</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>45656</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>45657</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>45659</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>45660</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>45664</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>45665</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
+        <v>45667</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
+        <v>45671</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
+        <v>45672</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
+        <v>45681</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
+        <v>45688</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
+        <v>45696</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
+        <v>45701</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
+        <v>45702</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
+        <v>45705</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="10">
+        <v>45707</v>
+      </c>
+      <c r="B36" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>45708</v>
+      </c>
+      <c r="B37" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="14"/>
+      <c r="B38" s="14">
+        <f>SUM(B2:B37)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>